<commit_message>
It's aint much but it is honest work
</commit_message>
<xml_diff>
--- a/example_lib.xlsx
+++ b/example_lib.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dom\Desktop\One_drive_folder\OneDrive - Uniwersytet Jagielloński\studemt\III Semestr\Python\Ćwiczenia\PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE514CE-3F81-4CE9-B244-808B72D6BBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417B685E-5719-4074-8BDE-4EA95F822756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>side_title</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>Lalka</t>
   </si>
   <si>
-    <t>Czyli ostatni zajazd na Litwie</t>
-  </si>
-  <si>
     <t>Adam</t>
   </si>
   <si>
@@ -88,6 +82,16 @@
   </si>
   <si>
     <t>Herling-Grudziński</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>yeahLorem ipsum dolor sit amet, consectetur adipiscing elit. Aliquam tellus sem, sodales eget nibh venenatis, dictum laoreet leo. Curabitur eleifend tellus eget tortor consectetur egestas. Nullam finibus pellentesque elit non lacinia. Integer venenatis pellentesque turpis, sit amet faucibus lectus. Duis vitae lacus nisi. Ut maximus nisi quis posuere ultricies. Quisque eu massa ligula. Orci varius natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus. Cras faucibus laoreet nisl non pellentesque. Curabitur volutpat nisi ac varius rutrum. Suspendisse potenti.
+Aenean efficitur efficitur nisl faucibus scelerisque. Etiam mattis est eu volutpat tristique. Nullam vitae massa consectetur, fermentum elit eu, fringilla nunc. Vivamus ac consectetur purus. Nunc at sem sed odio volutpat tempus. Donec in semper est. Phasellus quis sollicitudin massa. Nullam turpis lorem, eleifend eu laoreet vitae, egestas et ipsum. Curabitur sagittis pharetra blandit. Phasellus posuere augue vitae enim dapibus vulputate.</t>
+  </si>
+  <si>
+    <t>yeahLorem ipsum dolor sit amet, consectetur adipiscing elit. Aliquam tellus sem, sodales eget nibh venenatis, dictum laoreet leo. Curabitur eleifend tellus eget tortor consectetur egestas. Nullam finibus pellentesque elit non lacinia. Integer venenatis pellentesque turpis, sit amet faucibus lectus. Duis vitae lacus nisi. Ut maximus nisi quis posuere ultricies. Quisque eu massa ligula. Orci varius natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus. Cras faucibus laoreet nisl non pellentesque. Curabitur volutpat nisi ac varius rutrum. Suspendisse potenti. Aenean efficitur efficitur nisl faucibus scelerisque. Etiam mattis est eu volutpat tristique. Nullam vitae massa consectetur, fermentum elit eu, fringilla nunc. Vivamus ac consectetur purus. Nunc at sem sed odio volutpat tempus. Donec in semper est. Phasellus quis sollicitudin massa. Nullam turpis lorem, eleifend eu laoreet vitae, egestas et ipsum. Curabitur sagittis pharetra blandit. Phasellus posuere augue vitae enim dapibus vulputate.</t>
   </si>
 </sst>
 </file>
@@ -123,8 +127,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -407,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -417,6 +424,7 @@
     <col min="3" max="3" width="27.7265625" customWidth="1"/>
     <col min="4" max="4" width="16.90625" customWidth="1"/>
     <col min="5" max="5" width="17.6328125" customWidth="1"/>
+    <col min="6" max="6" width="16.08984375" customWidth="1"/>
     <col min="7" max="7" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -425,88 +433,100 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="11" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>